<commit_message>
up data treemap: add hyperlink
</commit_message>
<xml_diff>
--- a/data/s.xlsx
+++ b/data/s.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylezhang/Documents/Agora.io/Code/Idea-Box/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F745B194-0184-B546-82A2-965008E119EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A46FA2-0887-4643-8257-75B95E720B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="760" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="247">
   <si>
     <t>C1</t>
   </si>
@@ -45,9 +45,6 @@
     <t>1v1 教学</t>
   </si>
   <si>
-    <t>Agora Flat 开源教室</t>
-  </si>
-  <si>
     <t>1对多小班课</t>
   </si>
   <si>
@@ -663,104 +660,173 @@
     <t>元宇宙（Metaverse）</t>
   </si>
   <si>
-    <t>灵动课堂</t>
-  </si>
-  <si>
-    <t>伯索云学堂</t>
-  </si>
-  <si>
-    <t>flaget虚拟在线自习室</t>
-  </si>
-  <si>
-    <t>踢米(Timing)</t>
-  </si>
-  <si>
-    <t>360 AI 网课助手</t>
-  </si>
-  <si>
-    <t>全美测评优巡</t>
-  </si>
-  <si>
-    <t>VIP陪练-乐器陪练平台</t>
-  </si>
-  <si>
-    <t>少儿在线编程童程在线</t>
-  </si>
-  <si>
-    <t>大力智能学习灯</t>
-  </si>
-  <si>
-    <t>闳宸科技智能笔</t>
-  </si>
-  <si>
-    <t>凝趣科技智能笔</t>
-  </si>
-  <si>
-    <t>声网语音通话 API</t>
-  </si>
-  <si>
-    <t>在线 K 歌房场</t>
-  </si>
-  <si>
-    <t>一起听歌吧</t>
-  </si>
-  <si>
     <t>一起创作音乐</t>
   </si>
   <si>
-    <t>一起创作音乐flat</t>
-  </si>
-  <si>
-    <t>世纪佳缘</t>
-  </si>
-  <si>
-    <t>声网视频通话 API</t>
-  </si>
-  <si>
-    <t>微光</t>
-  </si>
-  <si>
-    <t>窝窝</t>
-  </si>
-  <si>
-    <t>Horizon Worlds</t>
-  </si>
-  <si>
-    <t>Beat Saber</t>
-  </si>
-  <si>
-    <t>Sud 互动游戏平台</t>
-  </si>
-  <si>
-    <t>腾讯先锋</t>
-  </si>
-  <si>
-    <t>Nine Chronicles</t>
-  </si>
-  <si>
-    <t>元直播 MetaLive</t>
-  </si>
-  <si>
-    <t>AvatarX 智能虚拟人平台</t>
-  </si>
-  <si>
-    <t>VS·work 元宇宙引擎</t>
-  </si>
-  <si>
-    <t>元 K 歌 MetaKTV</t>
-  </si>
-  <si>
-    <t>元语聊 MetaChat</t>
-  </si>
-  <si>
-    <t>互动游戏 Meta Interactive Game</t>
+    <t>教育</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agora Flat 开源教室｜https://flat.whiteboard.agora.io/</t>
+  </si>
+  <si>
+    <t>Agora Flat 开源教室｜https://flat.whiteboard.agora.io/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">1v1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF24292F"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>教学</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵动课堂｜https://www.agora.io/cn/agora-flexible-classroom</t>
+  </si>
+  <si>
+    <t>灵动课堂｜https://www.agora.io/cn/agora-flexible-classroom</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>伯索云学堂｜https://www.agora.io/cn/marketplace/plaso</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>flaget虚拟在线自习室｜https://www.flaget.cn/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>360 AI 网课助手｜https://www.agora.io/cn/marketplace/360ai-assistant</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>全美测评优巡｜https://www.agora.io/cn/marketplace/aitestgo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIP陪练-乐器陪练平台｜https://apps.apple.com/cn/app/id1174747377</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>少儿在线编程童程在线｜https://www.61it.cn/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>大力智能学习灯｜https://www.dali.com.cn/products</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>闳宸科技智能笔｜https://www.hongchentech.com/#/Pen</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>凝趣科技智能笔｜https://www.eningqu.com/Q2pen.html</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>声网语音通话 API｜https://www.agora.io/cn/voicecall</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在线 K 歌房场｜https://github.com/AgoraIO-Usecase/Online-KTV</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>一起听歌吧｜http://music.alang.run/#/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>一起创作音乐flat｜https://flat.io/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>世纪佳缘｜https://www.jiayuan.com/live/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>声网视频通话 API｜https://www.agora.io/cn/videocall</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>微光｜http://www.vlightv.com/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>窝窝｜https://www.wewave.com.cn/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Horizon Worlds｜https://www.oculus.com/horizon-worlds/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beat Saber｜https://www.oculus.com/experiences/quest/2448060205267927</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>太空杀｜http://www.snsslmm.com/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼人杀｜https://langrensha.163.com/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sud 互动游戏平台｜https://www.agora.io/cn/marketplace/sud</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>腾讯先锋｜https://gamer.qq.com/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nine Chronicles｜https://nine-chronicles.com/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>元直播 MetaLive｜https://www.agora.io/cn/meta-live</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AvatarX 智能虚拟人平台｜https://www.faceunity.com/avatarx.html</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VS·work 元宇宙引擎｜https://www.vswork.com/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>元 K 歌 MetaKTV｜https://www.agora.io/cn/meta-ktv</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>元语聊 MetaChat｜https://www.agora.io/cn/meta-chat</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>互动游戏 Meta Interactive Game｜https://www.agora.io/cn/meta-igame</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <name val="等线"/>
@@ -801,6 +867,18 @@
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292F"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292F"/>
+      <name val="Helvetica"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -844,13 +922,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1166,17 +1245,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G10" sqref="G10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="16" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1193,13 +1272,13 @@
     </row>
     <row r="2" spans="1:3" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>211</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1210,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1218,10 +1297,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1229,10 +1308,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1240,10 +1319,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1251,10 +1330,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1262,10 +1341,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1273,10 +1352,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1284,10 +1363,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1295,10 +1374,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1306,10 +1385,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1320,7 +1399,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1331,7 +1410,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1341,9 +1420,7 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>216</v>
-      </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
@@ -1397,7 +1474,9 @@
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="3" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
@@ -1407,7 +1486,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1418,7 +1497,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1429,7 +1508,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1437,10 +1516,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>5</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1450,9 +1529,7 @@
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>218</v>
-      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
@@ -1578,7 +1655,9 @@
       <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="3" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
@@ -1588,7 +1667,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1596,10 +1675,10 @@
         <v>3</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1609,110 +1688,108 @@
       <c r="B43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>221</v>
-      </c>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>210</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>226</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>49</v>
@@ -1721,7 +1798,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>50</v>
@@ -1730,7 +1807,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>51</v>
@@ -1739,7 +1816,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>52</v>
@@ -1748,7 +1825,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>53</v>
@@ -1757,241 +1834,241 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="2"/>
+      <c r="C58" s="3" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>230</v>
-      </c>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="2"/>
+      <c r="C63" s="3" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>222</v>
-      </c>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="2"/>
+      <c r="C66" s="3" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>64</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>65</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="26" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="26" customHeight="1">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>233</v>
-      </c>
+      <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C75" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>235</v>
-      </c>
+      <c r="C79" s="2"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>74</v>
@@ -2000,7 +2077,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>75</v>
@@ -2009,7 +2086,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>76</v>
@@ -2018,7 +2095,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>77</v>
@@ -2027,7 +2104,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>78</v>
@@ -2036,7 +2113,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>79</v>
@@ -2045,7 +2122,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>80</v>
@@ -2054,65 +2131,65 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C87" s="2"/>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" ht="26" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C88" s="2"/>
     </row>
-    <row r="89" spans="1:3" ht="26" customHeight="1">
+    <row r="89" spans="1:3">
       <c r="A89" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C89" s="2"/>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="C89" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="26" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="26" customHeight="1">
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C91" s="2"/>
+      <c r="C91" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>236</v>
-      </c>
+      <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>87</v>
@@ -2121,7 +2198,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>88</v>
@@ -2130,7 +2207,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>89</v>
@@ -2139,7 +2216,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>90</v>
@@ -2148,27 +2225,27 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C97" s="2"/>
+      <c r="C97" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>237</v>
-      </c>
+      <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>93</v>
@@ -2177,7 +2254,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>94</v>
@@ -2186,27 +2263,27 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C101" s="2"/>
+      <c r="C101" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>237</v>
-      </c>
+      <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>97</v>
@@ -2215,16 +2292,16 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="2" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>100</v>
@@ -2233,7 +2310,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>101</v>
@@ -2242,7 +2319,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>102</v>
@@ -2251,7 +2328,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>103</v>
@@ -2260,7 +2337,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>104</v>
@@ -2269,7 +2346,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>105</v>
@@ -2278,7 +2355,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>106</v>
@@ -2287,7 +2364,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>107</v>
@@ -2296,7 +2373,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>108</v>
@@ -2305,7 +2382,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>109</v>
@@ -2314,7 +2391,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>110</v>
@@ -2323,7 +2400,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>111</v>
@@ -2332,7 +2409,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>112</v>
@@ -2341,25 +2418,25 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C118" s="2"/>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" ht="26" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C119" s="2"/>
     </row>
-    <row r="120" spans="1:3" ht="26" customHeight="1">
+    <row r="120" spans="1:3">
       <c r="A120" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>115</v>
@@ -2368,7 +2445,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>116</v>
@@ -2377,7 +2454,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>117</v>
@@ -2386,7 +2463,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>118</v>
@@ -2395,7 +2472,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>119</v>
@@ -2404,7 +2481,7 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>120</v>
@@ -2413,7 +2490,7 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>121</v>
@@ -2422,7 +2499,7 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>122</v>
@@ -2431,7 +2508,7 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>123</v>
@@ -2440,7 +2517,7 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>124</v>
@@ -2449,7 +2526,7 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>125</v>
@@ -2458,7 +2535,7 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>126</v>
@@ -2467,16 +2544,16 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="2" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C132" s="2"/>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>129</v>
@@ -2485,7 +2562,7 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>130</v>
@@ -2494,7 +2571,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>131</v>
@@ -2503,7 +2580,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>132</v>
@@ -2512,7 +2589,7 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>133</v>
@@ -2521,7 +2598,7 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>134</v>
@@ -2530,7 +2607,7 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>135</v>
@@ -2539,25 +2616,25 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C140" s="2"/>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" ht="26" customHeight="1">
       <c r="A141" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C141" s="2"/>
     </row>
-    <row r="142" spans="1:3" ht="26" customHeight="1">
+    <row r="142" spans="1:3">
       <c r="A142" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>138</v>
@@ -2566,7 +2643,7 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>139</v>
@@ -2575,7 +2652,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>140</v>
@@ -2584,7 +2661,7 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>141</v>
@@ -2593,7 +2670,7 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>142</v>
@@ -2602,7 +2679,7 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>143</v>
@@ -2611,16 +2688,16 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C148" s="2"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>146</v>
@@ -2629,7 +2706,7 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>147</v>
@@ -2638,7 +2715,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>148</v>
@@ -2647,25 +2724,25 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C152" s="2"/>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" ht="26" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C153" s="2"/>
     </row>
-    <row r="154" spans="1:3" ht="26" customHeight="1">
+    <row r="154" spans="1:3">
       <c r="A154" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>151</v>
@@ -2674,7 +2751,7 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>152</v>
@@ -2683,7 +2760,7 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>153</v>
@@ -2692,7 +2769,7 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>154</v>
@@ -2701,7 +2778,7 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>155</v>
@@ -2710,7 +2787,7 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>156</v>
@@ -2719,7 +2796,7 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>157</v>
@@ -2728,7 +2805,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>158</v>
@@ -2737,7 +2814,7 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>159</v>
@@ -2746,16 +2823,16 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="2" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B163" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C163" s="2"/>
+    </row>
+    <row r="164" spans="1:3" ht="26" customHeight="1">
+      <c r="A164" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="C163" s="2"/>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>162</v>
@@ -2764,7 +2841,7 @@
     </row>
     <row r="165" spans="1:3" ht="26" customHeight="1">
       <c r="A165" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>163</v>
@@ -2773,7 +2850,7 @@
     </row>
     <row r="166" spans="1:3" ht="26" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>164</v>
@@ -2782,7 +2859,7 @@
     </row>
     <row r="167" spans="1:3" ht="26" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>165</v>
@@ -2791,7 +2868,7 @@
     </row>
     <row r="168" spans="1:3" ht="26" customHeight="1">
       <c r="A168" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>166</v>
@@ -2800,7 +2877,7 @@
     </row>
     <row r="169" spans="1:3" ht="26" customHeight="1">
       <c r="A169" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>167</v>
@@ -2809,7 +2886,7 @@
     </row>
     <row r="170" spans="1:3" ht="26" customHeight="1">
       <c r="A170" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>168</v>
@@ -2818,7 +2895,7 @@
     </row>
     <row r="171" spans="1:3" ht="26" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>169</v>
@@ -2827,7 +2904,7 @@
     </row>
     <row r="172" spans="1:3" ht="26" customHeight="1">
       <c r="A172" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>170</v>
@@ -2836,7 +2913,7 @@
     </row>
     <row r="173" spans="1:3" ht="26" customHeight="1">
       <c r="A173" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>171</v>
@@ -2845,16 +2922,16 @@
     </row>
     <row r="174" spans="1:3" ht="26" customHeight="1">
       <c r="A174" s="2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C174" s="2"/>
     </row>
     <row r="175" spans="1:3" ht="26" customHeight="1">
       <c r="A175" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>174</v>
@@ -2863,7 +2940,7 @@
     </row>
     <row r="176" spans="1:3" ht="26" customHeight="1">
       <c r="A176" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>175</v>
@@ -2872,7 +2949,7 @@
     </row>
     <row r="177" spans="1:3" ht="26" customHeight="1">
       <c r="A177" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>176</v>
@@ -2881,7 +2958,7 @@
     </row>
     <row r="178" spans="1:3" ht="26" customHeight="1">
       <c r="A178" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>177</v>
@@ -2890,7 +2967,7 @@
     </row>
     <row r="179" spans="1:3" ht="26" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>178</v>
@@ -2899,7 +2976,7 @@
     </row>
     <row r="180" spans="1:3" ht="26" customHeight="1">
       <c r="A180" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>179</v>
@@ -2908,7 +2985,7 @@
     </row>
     <row r="181" spans="1:3" ht="26" customHeight="1">
       <c r="A181" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>180</v>
@@ -2917,7 +2994,7 @@
     </row>
     <row r="182" spans="1:3" ht="26" customHeight="1">
       <c r="A182" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>181</v>
@@ -2926,7 +3003,7 @@
     </row>
     <row r="183" spans="1:3" ht="26" customHeight="1">
       <c r="A183" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>182</v>
@@ -2935,7 +3012,7 @@
     </row>
     <row r="184" spans="1:3" ht="26" customHeight="1">
       <c r="A184" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>183</v>
@@ -2944,7 +3021,7 @@
     </row>
     <row r="185" spans="1:3" ht="26" customHeight="1">
       <c r="A185" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>184</v>
@@ -2953,7 +3030,7 @@
     </row>
     <row r="186" spans="1:3" ht="26" customHeight="1">
       <c r="A186" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>185</v>
@@ -2962,7 +3039,7 @@
     </row>
     <row r="187" spans="1:3" ht="26" customHeight="1">
       <c r="A187" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>186</v>
@@ -2971,7 +3048,7 @@
     </row>
     <row r="188" spans="1:3" ht="26" customHeight="1">
       <c r="A188" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>187</v>
@@ -2980,7 +3057,7 @@
     </row>
     <row r="189" spans="1:3" ht="26" customHeight="1">
       <c r="A189" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>188</v>
@@ -2989,16 +3066,16 @@
     </row>
     <row r="190" spans="1:3" ht="26" customHeight="1">
       <c r="A190" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>189</v>
       </c>
       <c r="C190" s="2"/>
     </row>
-    <row r="191" spans="1:3" ht="26" customHeight="1">
+    <row r="191" spans="1:3">
       <c r="A191" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>190</v>
@@ -3007,7 +3084,7 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>191</v>
@@ -3016,7 +3093,7 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>192</v>
@@ -3025,25 +3102,25 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C194" s="2"/>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" ht="26" customHeight="1">
       <c r="A195" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C195" s="2"/>
     </row>
-    <row r="196" spans="1:3" ht="26" customHeight="1">
+    <row r="196" spans="1:3">
       <c r="A196" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>195</v>
@@ -3052,7 +3129,7 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>196</v>
@@ -3061,7 +3138,7 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>197</v>
@@ -3070,7 +3147,7 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>198</v>
@@ -3079,7 +3156,7 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>199</v>
@@ -3088,16 +3165,16 @@
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="2" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C201" s="2"/>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>202</v>
@@ -3106,27 +3183,27 @@
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C203" s="2"/>
+      <c r="C203" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C204" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="C204" s="2"/>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>205</v>
@@ -3135,7 +3212,7 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>206</v>
@@ -3144,7 +3221,7 @@
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>207</v>
@@ -3153,7 +3230,7 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>208</v>
@@ -3162,117 +3239,94 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C209" s="2"/>
+      <c r="C209" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://flat.whiteboard.agora.io/" xr:uid="{5F86872E-F2BE-A146-BA24-4EF24E7D6B8F}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://www.agora.io/cn/agora-flexible-classroom" xr:uid="{14B33CC1-F0D7-FC45-BEA9-CBC0B57AFD14}"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://flat.whiteboard.agora.io/" xr:uid="{13EB8382-E581-D44F-8AE0-802F5DD8F362}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://www.agora.io/cn/agora-flexible-classroom" xr:uid="{154C4666-A17D-F842-BD99-C6E3C6B91B23}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://flat.whiteboard.agora.io/" xr:uid="{65CDE110-2D40-A242-A593-AA74552520E0}"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://www.agora.io/cn/agora-flexible-classroom" xr:uid="{13E406C1-1C47-DC45-BBEB-ED6735700583}"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://flat.whiteboard.agora.io/" xr:uid="{E3567B2E-551A-224E-B51A-444208AB7FB9}"/>
-    <hyperlink ref="C9" r:id="rId8" display="https://www.agora.io/cn/agora-flexible-classroom" xr:uid="{77674504-870B-BE4D-A893-617141282211}"/>
-    <hyperlink ref="C10" r:id="rId9" display="https://www.agora.io/cn/marketplace/plaso" xr:uid="{5A6D17F7-F569-AC44-B6AA-E3781235E98E}"/>
-    <hyperlink ref="C11" r:id="rId10" display="https://flat.whiteboard.agora.io/" xr:uid="{CAA302D3-42E9-A046-AB9E-421193E8AF45}"/>
-    <hyperlink ref="C12" r:id="rId11" display="https://www.flaget.cn/" xr:uid="{3A3F0BB0-A666-4A4D-83F2-E0F64A169BC3}"/>
-    <hyperlink ref="C13" r:id="rId12" display="http://www.huiian.com/" xr:uid="{CAF273F1-4D9C-A44F-B70A-DF953F82BCF7}"/>
-    <hyperlink ref="C14" r:id="rId13" display="https://www.agora.io/cn/marketplace/360ai-assistant" xr:uid="{72370C3C-7A96-2942-9702-A7215DB26D8B}"/>
-    <hyperlink ref="C15" r:id="rId14" display="https://www.agora.io/cn/marketplace/aitestgo" xr:uid="{72527E1E-C188-4646-8350-36D1DC7D5AF5}"/>
-    <hyperlink ref="C22" r:id="rId15" display="https://apps.apple.com/cn/app/id1174747377" xr:uid="{CAA046B9-6C8E-3647-81C1-CCEDE117D618}"/>
-    <hyperlink ref="C23" r:id="rId16" display="https://flat.whiteboard.agora.io/" xr:uid="{5C448340-B975-D549-A36B-4859C64E1DEA}"/>
-    <hyperlink ref="C24" r:id="rId17" display="https://flat.whiteboard.agora.io/" xr:uid="{369A4189-7C84-C94B-9985-A2E07D2D26F4}"/>
-    <hyperlink ref="C25" r:id="rId18" display="https://flat.whiteboard.agora.io/" xr:uid="{39C9FE62-0527-8147-84AE-3422F42AA78C}"/>
-    <hyperlink ref="C26" r:id="rId19" display="https://www.61it.cn/" xr:uid="{607B2322-D8B7-3947-826E-550A270E37C4}"/>
-    <hyperlink ref="C41" r:id="rId20" display="https://www.dali.com.cn/products" xr:uid="{0A1A1CDE-29E3-574D-8B9A-5FE924D7CB44}"/>
-    <hyperlink ref="C42" r:id="rId21" location="/Pen" display="https://www.hongchentech.com/ - /Pen" xr:uid="{52FA05C9-BE0A-714C-A306-48A8E64DE248}"/>
-    <hyperlink ref="C43" r:id="rId22" display="https://www.eningqu.com/Q2pen.html" xr:uid="{3E2E5BEA-93D0-7444-9674-D7C89C6440C7}"/>
-    <hyperlink ref="C45" r:id="rId23" display="https://www.agora.io/cn/voicecall" xr:uid="{57EDE8D9-3E90-0D41-B78A-ACA9E06B826D}"/>
-    <hyperlink ref="C46" r:id="rId24" display="https://www.agora.io/cn/voicecall" xr:uid="{C3466EDD-EFEC-1744-B655-EFBBF55F709E}"/>
-    <hyperlink ref="C47" r:id="rId25" display="https://www.agora.io/cn/voicecall" xr:uid="{85E433F0-A50D-6848-BC3E-4BE73267F965}"/>
-    <hyperlink ref="C48" r:id="rId26" display="https://www.agora.io/cn/voicecall" xr:uid="{F0BEBC97-49D8-7548-911B-B9833E690AA3}"/>
-    <hyperlink ref="C49" r:id="rId27" display="https://www.agora.io/cn/voicecall" xr:uid="{511DD163-5CF0-4148-9D54-3B0C3568F415}"/>
-    <hyperlink ref="C50" r:id="rId28" display="https://github.com/AgoraIO-Usecase/Online-KTV" xr:uid="{41798F69-E115-9C44-9739-C2330B578650}"/>
-    <hyperlink ref="C51" r:id="rId29" location="/" display="http://music.alang.run/ - /" xr:uid="{624EA99F-9ECE-CD43-8947-93A6EA5ACCCF}"/>
-    <hyperlink ref="C52" r:id="rId30" display="https://flat.io/" xr:uid="{2421F4E0-0622-014C-9F2C-6BFAD98D532B}"/>
-    <hyperlink ref="C59" r:id="rId31" display="https://www.jiayuan.com/live/" xr:uid="{C750301C-FF90-AC46-B0E1-108EF88B13A2}"/>
-    <hyperlink ref="C60" r:id="rId32" display="https://www.agora.io/cn/videocall" xr:uid="{B4C22991-A1A7-5D4F-9FE3-A2B1C5913E90}"/>
-    <hyperlink ref="C61" r:id="rId33" display="http://www.vlightv.com/" xr:uid="{7D1C76C6-5683-6448-B618-0A51AEBE362A}"/>
-    <hyperlink ref="C62" r:id="rId34" display="https://www.wewave.com.cn/" xr:uid="{3A73D258-DD5F-8B4A-96A3-CC18D937FA5D}"/>
-    <hyperlink ref="C64" r:id="rId35" display="https://www.oculus.com/horizon-worlds/" xr:uid="{7271DE77-CA0D-C149-8909-D080DA14E32B}"/>
-    <hyperlink ref="C65" r:id="rId36" display="https://www.agora.io/cn/voicecall" xr:uid="{8A67D7D4-0A09-0349-A4D8-820FCF67D20A}"/>
-    <hyperlink ref="C67" r:id="rId37" display="https://www.oculus.com/experiences/quest/2448060205267927" xr:uid="{10F2D68B-62DD-CB49-9F59-7FF9947A192F}"/>
-    <hyperlink ref="C68" r:id="rId38" display="https://www.agora.io/cn/voicecall" xr:uid="{A3CF83E8-03A7-934F-BF8A-A2F30D5EB124}"/>
-    <hyperlink ref="C69" r:id="rId39" display="http://www.snsslmm.com/" xr:uid="{40FB46F0-3368-FF44-9A3C-56D197F817D1}"/>
-    <hyperlink ref="C70" r:id="rId40" display="https://langrensha.163.com/" xr:uid="{50FD3608-186C-B84B-B94B-9C22B77C2068}"/>
-    <hyperlink ref="C71" r:id="rId41" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{A3A7421E-F904-A349-B40A-92B4069B4909}"/>
-    <hyperlink ref="C72" r:id="rId42" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{F8AA91D3-A696-9041-BA77-067BB05E66DD}"/>
-    <hyperlink ref="C73" r:id="rId43" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{6CE55C13-DB4B-284D-B6CE-6E4306A6E1D0}"/>
-    <hyperlink ref="C74" r:id="rId44" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{75B43CE5-7942-5944-9239-1BB4E73CDF28}"/>
-    <hyperlink ref="C76" r:id="rId45" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{D42D2829-A2F2-1C4F-ABC2-25BFFAB0BD2C}"/>
-    <hyperlink ref="C77" r:id="rId46" display="https://gamer.qq.com/" xr:uid="{D5F52692-D863-154A-AE15-DC131525AE65}"/>
-    <hyperlink ref="C78" r:id="rId47" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{C5897DE0-5992-2541-9EEA-932083DE8409}"/>
-    <hyperlink ref="C79" r:id="rId48" display="https://nine-chronicles.com/" xr:uid="{C121F324-6873-0B43-A36C-416979156206}"/>
-    <hyperlink ref="C90" r:id="rId49" display="https://www.agora.io/cn/meta-live" xr:uid="{49C7BA2B-D7CC-1045-BD6B-E70811F6E77E}"/>
-    <hyperlink ref="C92" r:id="rId50" display="https://www.agora.io/cn/meta-live" xr:uid="{261B7C99-2915-284C-A436-C075A56A89B5}"/>
-    <hyperlink ref="C98" r:id="rId51" display="https://www.faceunity.com/avatarx.html" xr:uid="{DAFF9367-B0F5-404B-9F9C-A0A96D2F5CEB}"/>
-    <hyperlink ref="C102" r:id="rId52" display="https://www.faceunity.com/avatarx.html" xr:uid="{3A4EDEF8-47E4-0542-9437-03FE5080BBF3}"/>
-    <hyperlink ref="C204" r:id="rId53" display="https://www.vswork.com/" xr:uid="{61903FB1-2813-BC4F-AC4C-9B601298296A}"/>
-    <hyperlink ref="C210" r:id="rId54" display="https://www.agora.io/cn/meta-ktv" xr:uid="{25316486-1C0F-D544-B8F0-85BCFB62E3CF}"/>
-    <hyperlink ref="C211" r:id="rId55" display="https://www.agora.io/cn/meta-chat" xr:uid="{5257A025-68E8-CA4D-802E-6976C90F5CD0}"/>
-    <hyperlink ref="C212" r:id="rId56" display="https://www.agora.io/cn/meta-igame" xr:uid="{A2AD1B48-5B2F-A540-9723-9A1E6B3C5509}"/>
-    <hyperlink ref="C213" r:id="rId57" display="https://www.agora.io/cn/meta-live" xr:uid="{C1C2DD2B-27A5-B04D-9556-8E3388179B95}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.agora.io/cn/agora-flexible-classroom" xr:uid="{14B33CC1-F0D7-FC45-BEA9-CBC0B57AFD14}"/>
+    <hyperlink ref="C10" r:id="rId2" display="https://www.agora.io/cn/marketplace/plaso" xr:uid="{5A6D17F7-F569-AC44-B6AA-E3781235E98E}"/>
+    <hyperlink ref="C12" r:id="rId3" display="https://www.flaget.cn/" xr:uid="{3A3F0BB0-A666-4A4D-83F2-E0F64A169BC3}"/>
+    <hyperlink ref="C13" r:id="rId4" display="https://www.agora.io/cn/marketplace/360ai-assistant" xr:uid="{72370C3C-7A96-2942-9702-A7215DB26D8B}"/>
+    <hyperlink ref="C14" r:id="rId5" display="https://www.agora.io/cn/marketplace/aitestgo" xr:uid="{72527E1E-C188-4646-8350-36D1DC7D5AF5}"/>
+    <hyperlink ref="C21" r:id="rId6" display="https://apps.apple.com/cn/app/id1174747377" xr:uid="{CAA046B9-6C8E-3647-81C1-CCEDE117D618}"/>
+    <hyperlink ref="C25" r:id="rId7" display="https://www.61it.cn/" xr:uid="{607B2322-D8B7-3947-826E-550A270E37C4}"/>
+    <hyperlink ref="C40" r:id="rId8" display="https://www.dali.com.cn/products" xr:uid="{0A1A1CDE-29E3-574D-8B9A-5FE924D7CB44}"/>
+    <hyperlink ref="C41" r:id="rId9" location="/Pen" display="https://www.hongchentech.com/ - /Pen" xr:uid="{52FA05C9-BE0A-714C-A306-48A8E64DE248}"/>
+    <hyperlink ref="C42" r:id="rId10" display="https://www.eningqu.com/Q2pen.html" xr:uid="{3E2E5BEA-93D0-7444-9674-D7C89C6440C7}"/>
+    <hyperlink ref="C44" r:id="rId11" display="https://www.agora.io/cn/voicecall" xr:uid="{57EDE8D9-3E90-0D41-B78A-ACA9E06B826D}"/>
+    <hyperlink ref="C49" r:id="rId12" display="https://github.com/AgoraIO-Usecase/Online-KTV" xr:uid="{41798F69-E115-9C44-9739-C2330B578650}"/>
+    <hyperlink ref="C50" r:id="rId13" location="/" display="http://music.alang.run/ - /" xr:uid="{624EA99F-9ECE-CD43-8947-93A6EA5ACCCF}"/>
+    <hyperlink ref="C51" r:id="rId14" display="https://flat.io/" xr:uid="{2421F4E0-0622-014C-9F2C-6BFAD98D532B}"/>
+    <hyperlink ref="C58" r:id="rId15" display="https://www.jiayuan.com/live/" xr:uid="{C750301C-FF90-AC46-B0E1-108EF88B13A2}"/>
+    <hyperlink ref="C59" r:id="rId16" display="https://www.agora.io/cn/videocall" xr:uid="{B4C22991-A1A7-5D4F-9FE3-A2B1C5913E90}"/>
+    <hyperlink ref="C60" r:id="rId17" display="http://www.vlightv.com/" xr:uid="{7D1C76C6-5683-6448-B618-0A51AEBE362A}"/>
+    <hyperlink ref="C61" r:id="rId18" display="https://www.wewave.com.cn/" xr:uid="{3A73D258-DD5F-8B4A-96A3-CC18D937FA5D}"/>
+    <hyperlink ref="C63" r:id="rId19" display="https://www.oculus.com/horizon-worlds/" xr:uid="{7271DE77-CA0D-C149-8909-D080DA14E32B}"/>
+    <hyperlink ref="C66" r:id="rId20" display="https://www.oculus.com/experiences/quest/2448060205267927" xr:uid="{10F2D68B-62DD-CB49-9F59-7FF9947A192F}"/>
+    <hyperlink ref="C68" r:id="rId21" display="http://www.snsslmm.com/" xr:uid="{40FB46F0-3368-FF44-9A3C-56D197F817D1}"/>
+    <hyperlink ref="C69" r:id="rId22" display="https://langrensha.163.com/" xr:uid="{50FD3608-186C-B84B-B94B-9C22B77C2068}"/>
+    <hyperlink ref="C70" r:id="rId23" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{A3A7421E-F904-A349-B40A-92B4069B4909}"/>
+    <hyperlink ref="C76" r:id="rId24" display="https://gamer.qq.com/" xr:uid="{D5F52692-D863-154A-AE15-DC131525AE65}"/>
+    <hyperlink ref="C78" r:id="rId25" display="https://nine-chronicles.com/" xr:uid="{C121F324-6873-0B43-A36C-416979156206}"/>
+    <hyperlink ref="C89" r:id="rId26" display="https://www.agora.io/cn/meta-live" xr:uid="{49C7BA2B-D7CC-1045-BD6B-E70811F6E77E}"/>
+    <hyperlink ref="C97" r:id="rId27" display="https://www.faceunity.com/avatarx.html" xr:uid="{DAFF9367-B0F5-404B-9F9C-A0A96D2F5CEB}"/>
+    <hyperlink ref="C101" r:id="rId28" display="https://www.faceunity.com/avatarx.html" xr:uid="{3A4EDEF8-47E4-0542-9437-03FE5080BBF3}"/>
+    <hyperlink ref="C203" r:id="rId29" display="https://www.vswork.com/" xr:uid="{61903FB1-2813-BC4F-AC4C-9B601298296A}"/>
+    <hyperlink ref="C209" r:id="rId30" display="https://www.agora.io/cn/meta-ktv" xr:uid="{25316486-1C0F-D544-B8F0-85BCFB62E3CF}"/>
+    <hyperlink ref="C210" r:id="rId31" display="https://www.agora.io/cn/meta-chat" xr:uid="{5257A025-68E8-CA4D-802E-6976C90F5CD0}"/>
+    <hyperlink ref="C211" r:id="rId32" display="https://www.agora.io/cn/meta-igame" xr:uid="{A2AD1B48-5B2F-A540-9723-9A1E6B3C5509}"/>
+    <hyperlink ref="C212" r:id="rId33" display="https://www.agora.io/cn/meta-live" xr:uid="{C1C2DD2B-27A5-B04D-9556-8E3388179B95}"/>
+    <hyperlink ref="C2" r:id="rId34" display="https://flat.whiteboard.agora.io/" xr:uid="{5F86872E-F2BE-A146-BA24-4EF24E7D6B8F}"/>
+    <hyperlink ref="C5" r:id="rId35" display="https://www.agora.io/cn/agora-flexible-classroom" xr:uid="{7763AE2F-F06F-D44C-9C19-BBDDED6E8274}"/>
+    <hyperlink ref="C4" r:id="rId36" display="https://flat.whiteboard.agora.io/" xr:uid="{244AE708-8A28-8842-B232-54ACC2E1041D}"/>
+    <hyperlink ref="C45:C48" r:id="rId37" display="https://www.agora.io/cn/voicecall" xr:uid="{4A8B5DB8-FB94-5E44-A957-F75F1B8B711B}"/>
+    <hyperlink ref="C64" r:id="rId38" display="https://www.agora.io/cn/voicecall" xr:uid="{08D1B1F5-6694-0145-A538-17A4A2FE70E4}"/>
+    <hyperlink ref="C67" r:id="rId39" display="https://www.agora.io/cn/voicecall" xr:uid="{5477C597-55F0-C745-B80E-709BAE86DDFD}"/>
+    <hyperlink ref="C71:C73" r:id="rId40" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{0D6C1EB1-EE49-5A4A-874D-96E2CB9EF058}"/>
+    <hyperlink ref="C75" r:id="rId41" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{990A42D2-473C-8345-AB4C-B02C87C541D9}"/>
+    <hyperlink ref="C77" r:id="rId42" display="https://www.agora.io/cn/marketplace/sud" xr:uid="{AC78B4FE-1232-084E-AD86-63391D41608E}"/>
+    <hyperlink ref="C91" r:id="rId43" display="https://www.agora.io/cn/meta-live" xr:uid="{34C875FF-2E6D-E94B-8911-3138844BDFF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update site and data
</commit_message>
<xml_diff>
--- a/data/s.xlsx
+++ b/data/s.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylezhang/Documents/Agora.io/Code/Idea-Box/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E216FC5-95F6-2442-A25B-1D55364828FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106749BC-9AE2-8E44-B91D-50FFCC33A891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="760" windowWidth="29340" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1502,7 +1502,7 @@
   <dimension ref="A1:D219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>